<commit_message>
work on config panel for trigger options
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_29_Apr.xlsx
+++ b/other/Project_TimeLine_2021_29_Apr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6A1E16-9AA0-4848-B0D5-CDBC4A753E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15084F4F-64D8-4A88-AF60-8BC8F5F81875}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>S/N</t>
   </si>
@@ -151,13 +151,6 @@
   </si>
   <si>
     <t>Front-end: Threejs scene - Colour grouping</t>
-  </si>
-  <si>
-    <t>Front-end: Threejs scene - MQTT client</t>
-  </si>
-  <si>
-    <t>reordered to complete
-group features first</t>
   </si>
   <si>
     <t>Completed:
@@ -554,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1059,7 @@
         <v>44301</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I21" s="4"/>
     </row>
@@ -1117,7 +1110,7 @@
         <v>44306</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1139,9 +1132,7 @@
       <c r="G24" s="3">
         <v>44308</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1164,24 +1155,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" s="3">
-        <v>44316</v>
-      </c>
-      <c r="F26" s="3">
-        <v>44319</v>
-      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>

</xml_diff>

<commit_message>
documentation update, running npm update after this
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_29_Apr.xlsx
+++ b/other/Project_TimeLine_2021_29_Apr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15084F4F-64D8-4A88-AF60-8BC8F5F81875}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A043DBD2-04C2-4FC3-B422-1EE1BFDD04B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -164,7 +164,8 @@
 - edit group id
 - edit group colours
 - select by group id
-- light name overlay on screen (toggleable)</t>
+- light name overlay on screen (toggleable)
+- adding/removing triggers</t>
   </si>
 </sst>
 </file>
@@ -548,7 +549,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1037,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>

</xml_diff>